<commit_message>
修复 Streamlit Cloud 依赖问题
</commit_message>
<xml_diff>
--- a/PACKING_LIST_2024-00-90868.xlsx
+++ b/PACKING_LIST_2024-00-90868.xlsx
@@ -1375,7 +1375,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:ABC105"/>
+  <dimension ref="A1:IV105"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="116" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
@@ -1772,11 +1772,6 @@
       <c r="P17" t="n">
         <v>250</v>
       </c>
-      <c r="ABC17" t="inlineStr">
-        <is>
-          <t>BHB10712-CLRK</t>
-        </is>
-      </c>
     </row>
     <row r="18" ht="24" customFormat="1" customHeight="1" s="56">
       <c r="A18" s="25" t="inlineStr">
@@ -1821,11 +1816,6 @@
       <c r="P18" t="n">
         <v>250</v>
       </c>
-      <c r="ABC18" t="inlineStr">
-        <is>
-          <t>BHB8510-CLRK</t>
-        </is>
-      </c>
     </row>
     <row r="19" ht="24" customFormat="1" customHeight="1" s="56">
       <c r="A19" s="25" t="inlineStr">
@@ -1869,11 +1859,6 @@
       </c>
       <c r="P19" s="56" t="n">
         <v>200</v>
-      </c>
-      <c r="ABC19" t="inlineStr">
-        <is>
-          <t>BHB141016-CLRK</t>
-        </is>
       </c>
     </row>
     <row r="20" ht="24" customFormat="1" customHeight="1" s="56">

</xml_diff>